<commit_message>
Added all game images
</commit_message>
<xml_diff>
--- a/Game Categories.xlsx
+++ b/Game Categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badr\Documents\GitHub\GameRecommApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D04641-91F4-4279-A816-EBB9F9877BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED4400C-86C1-4E2B-8911-361A7D22C7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5508" yWindow="2112" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t xml:space="preserve">animal crossing </t>
   </si>
   <si>
-    <t>fifa 2024</t>
-  </si>
-  <si>
     <t>cyberpunk 2077</t>
   </si>
   <si>
@@ -298,6 +295,9 @@
   </si>
   <si>
     <t>short, medium</t>
+  </si>
+  <si>
+    <t>FC 24</t>
   </si>
 </sst>
 </file>
@@ -639,8 +639,8 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O39" sqref="O39"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,49 +650,49 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="I1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="O1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -700,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -712,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -724,30 +724,30 @@
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M2" s="3">
         <v>0</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -771,22 +771,22 @@
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -806,7 +806,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -818,30 +818,30 @@
         <v>1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M4" s="3">
         <v>1</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -853,7 +853,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
@@ -865,22 +865,22 @@
         <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M5" s="1">
         <v>1</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -888,7 +888,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -900,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="3">
         <v>1</v>
@@ -912,22 +912,22 @@
         <v>1</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M6" s="3">
         <v>0</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -935,7 +935,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -959,30 +959,30 @@
         <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M7" s="1">
         <v>1</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -1006,30 +1006,30 @@
         <v>0</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M8" s="3">
         <v>1</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -1041,7 +1041,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
@@ -1053,30 +1053,30 @@
         <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -1088,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
@@ -1100,30 +1100,30 @@
         <v>0</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M10" s="3">
         <v>1</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -1135,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
@@ -1147,30 +1147,30 @@
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M11" s="1">
-        <v>1</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -1182,7 +1182,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="3">
         <v>1</v>
@@ -1194,30 +1194,30 @@
         <v>0</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M12" s="3">
         <v>0</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -1229,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -1241,30 +1241,30 @@
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M13" s="1">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -1276,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="3">
         <v>1</v>
@@ -1288,30 +1288,30 @@
         <v>1</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M14" s="3">
         <v>0</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1323,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
@@ -1335,30 +1335,30 @@
         <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M15" s="1">
         <v>0</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" s="3">
         <v>1</v>
@@ -1382,30 +1382,30 @@
         <v>0</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M16" s="3">
         <v>0</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -1417,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="1">
         <v>1</v>
@@ -1429,30 +1429,30 @@
         <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M17" s="1">
         <v>0</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -1464,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G18" s="1">
         <v>1</v>
@@ -1476,30 +1476,30 @@
         <v>1</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M18" s="1">
         <v>0</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -1511,7 +1511,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G19" s="1">
         <v>1</v>
@@ -1523,30 +1523,30 @@
         <v>1</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M19" s="1">
         <v>0</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -1558,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -1570,30 +1570,30 @@
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M20" s="1">
         <v>1</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -1605,7 +1605,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G21" s="1">
         <v>1</v>
@@ -1617,30 +1617,30 @@
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M21" s="1">
         <v>0</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -1652,7 +1652,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G22" s="1">
         <v>1</v>
@@ -1664,30 +1664,30 @@
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M22" s="1">
         <v>0</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -1699,7 +1699,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
@@ -1711,30 +1711,30 @@
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M23" s="1">
         <v>1</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -1746,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
@@ -1758,30 +1758,30 @@
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M24" s="1">
         <v>0</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -1793,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G25" s="1">
         <v>1</v>
@@ -1805,30 +1805,30 @@
         <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M25" s="1">
         <v>0</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -1840,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G26" s="1">
         <v>0</v>
@@ -1852,30 +1852,30 @@
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O26" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M26" s="1">
-        <v>1</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G27" s="1">
         <v>0</v>
@@ -1899,30 +1899,30 @@
         <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O27" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M27" s="1">
-        <v>1</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
@@ -1934,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G28" s="1">
         <v>1</v>
@@ -1946,30 +1946,30 @@
         <v>0</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M28" s="1">
         <v>0</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -1981,7 +1981,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
@@ -1993,30 +1993,30 @@
         <v>1</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M29" s="1">
         <v>0</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
@@ -2028,7 +2028,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G30" s="1">
         <v>0</v>
@@ -2040,30 +2040,30 @@
         <v>0</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M30" s="1">
         <v>1</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
@@ -2075,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G31" s="1">
         <v>1</v>
@@ -2087,30 +2087,30 @@
         <v>1</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M31" s="1">
         <v>0</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -2122,7 +2122,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G32" s="1">
         <v>0</v>
@@ -2134,30 +2134,30 @@
         <v>0</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M32" s="1">
         <v>1</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
@@ -2169,7 +2169,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G33" s="1">
         <v>0</v>
@@ -2181,30 +2181,30 @@
         <v>1</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M33" s="1">
+        <v>1</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O33" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M33" s="1">
-        <v>1</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -2216,7 +2216,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G34" s="1">
         <v>1</v>
@@ -2228,30 +2228,30 @@
         <v>0</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M34" s="1">
         <v>0</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G35" s="1">
         <v>0</v>
@@ -2275,30 +2275,30 @@
         <v>0</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M35" s="1">
         <v>1</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
@@ -2310,7 +2310,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G36" s="1">
         <v>1</v>
@@ -2322,30 +2322,30 @@
         <v>1</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M36" s="1">
         <v>1</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
@@ -2357,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G37" s="1">
         <v>1</v>
@@ -2369,30 +2369,30 @@
         <v>1</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M37" s="1">
         <v>0</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
@@ -2404,7 +2404,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G38" s="1">
         <v>1</v>
@@ -2416,22 +2416,22 @@
         <v>0</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M38" s="1">
         <v>0</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final version with new games added and all gmaes panel
</commit_message>
<xml_diff>
--- a/Game Categories.xlsx
+++ b/Game Categories.xlsx
@@ -1,19 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badr\Documents\GitHub\GameRecommApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\Year 2\Semester 2\Programming Languages Paradigms\Project\GameRecommApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED4400C-86C1-4E2B-8911-361A7D22C7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5508" yWindow="2112" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5508" yWindow="2112" windowWidth="17280" windowHeight="8880"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Game Categories" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="98">
   <si>
     <t>The Witcher 3</t>
   </si>
@@ -298,12 +297,33 @@
   </si>
   <si>
     <t>FC 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red Dead Redemption </t>
+  </si>
+  <si>
+    <t>Red Dead Redemption 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elden Ring </t>
+  </si>
+  <si>
+    <t>Elden Ring Nightreign</t>
+  </si>
+  <si>
+    <t>rpg, adventuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outlast </t>
+  </si>
+  <si>
+    <t>Outlast 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -635,12 +655,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2434,6 +2454,288 @@
         <v>51</v>
       </c>
     </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1">
+        <v>1</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M39" s="1">
+        <v>0</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1</v>
+      </c>
+      <c r="I40" s="1">
+        <v>1</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M40" s="1">
+        <v>0</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+      <c r="I41" s="1">
+        <v>1</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M41" s="1">
+        <v>0</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1">
+        <v>1</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M42" s="1">
+        <v>1</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0</v>
+      </c>
+      <c r="I43" s="1">
+        <v>1</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M43" s="1">
+        <v>0</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1">
+        <v>1</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M44" s="1">
+        <v>0</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>